<commit_message>
Remove reliance on CareLink for CNL hash and link encryption key
</commit_message>
<xml_diff>
--- a/Bayer-Medtronic-640G USB HID Interface.xlsx
+++ b/Bayer-Medtronic-640G USB HID Interface.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgoedhart/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennart/Documents/Remote Control Caty/decoding-contour-next-link/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="28280" windowHeight="16040" tabRatio="745"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="28280" windowHeight="16040" tabRatio="745" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="USB Packets" sheetId="11" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="OPEN_CONNECTION Request" sheetId="18" r:id="rId6"/>
     <sheet name="OPEN_CONNECTION Response" sheetId="17" r:id="rId7"/>
     <sheet name="READ_INFO Response" sheetId="15" r:id="rId8"/>
-    <sheet name="Negotiate Channel" sheetId="12" r:id="rId9"/>
-    <sheet name="SEND_MESSAGE Request" sheetId="23" r:id="rId10"/>
-    <sheet name="SEND_MESSAGE Response" sheetId="13" r:id="rId11"/>
-    <sheet name="RECEIVE_MESSAGE" sheetId="24" r:id="rId12"/>
+    <sheet name="REQUEST_LINK_KEY Response" sheetId="26" r:id="rId9"/>
+    <sheet name="Negotiate Channel" sheetId="12" r:id="rId10"/>
+    <sheet name="SEND_MESSAGE Request" sheetId="23" r:id="rId11"/>
+    <sheet name="SEND_MESSAGE Response" sheetId="13" r:id="rId12"/>
+    <sheet name="RECEIVE_MESSAGE" sheetId="24" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="194">
   <si>
     <t>Byte</t>
   </si>
@@ -91,9 +92,6 @@
     <t>09</t>
   </si>
   <si>
-    <t>FrameType</t>
-  </si>
-  <si>
     <t>1-3</t>
   </si>
   <si>
@@ -250,9 +248,6 @@
     <t>Payload length in bytes and over frames. Length &gt;27 means that payload continues in next incoming frame (1-n). Currently assuming a little-endian 4 byte unsigned int</t>
   </si>
   <si>
-    <t>Frame type sequence number. Currently assuming a little-endian 4 byte unsigned int</t>
-  </si>
-  <si>
     <t>N+1</t>
   </si>
   <si>
@@ -319,15 +314,6 @@
     <t>Command Action</t>
   </si>
   <si>
-    <t>0x55 - ("U") - Pump response</t>
-  </si>
-  <si>
-    <t>0x03 - Pump comms channel negotiate</t>
-  </si>
-  <si>
-    <t>0x05 - Pump request</t>
-  </si>
-  <si>
     <t>Medtronic message size. Size of the message body, from byte 1 until the end of the payload, but not including the CRC</t>
   </si>
   <si>
@@ -424,9 +410,6 @@
     <t>Pump SN</t>
   </si>
   <si>
-    <t>17-19</t>
-  </si>
-  <si>
     <t>Unknown bytes, currently assume always 0x00 padded</t>
   </si>
   <si>
@@ -589,9 +572,6 @@
     <t>Link MAC as a big-endian long</t>
   </si>
   <si>
-    <t>Pump MAC as a big-endian long</t>
-  </si>
-  <si>
     <t>Link MAC as a little-endian long</t>
   </si>
   <si>
@@ -605,6 +585,42 @@
   </si>
   <si>
     <t>Sequence Number as a little-endian 3 byte integer? 3 byte int seems unlikely, but that's best guess at this stage</t>
+  </si>
+  <si>
+    <t>Link Device Operation</t>
+  </si>
+  <si>
+    <t>Link Operation sequence number. Currently assuming a little-endian 4 byte unsigned int</t>
+  </si>
+  <si>
+    <t>Encryption Mode. 1 = on, 0 = off</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>Pump MAC as a big-endian long. If this is null padded, then this Next Link is not associated (paired) with the pump. If this is the case, you can do a Key Exchange for a temporary association</t>
+  </si>
+  <si>
+    <t>Current Link Counter as a little-endian short</t>
+  </si>
+  <si>
+    <t>0x03 - JOIN NETWORK COMMAND</t>
+  </si>
+  <si>
+    <t>0x05 - TRANSMIT PACKET</t>
+  </si>
+  <si>
+    <t>0x55 - ("U") - PACKET RESPONSE HEADER</t>
+  </si>
+  <si>
+    <t>Contained by: One Bayer Binary Message (Frame Type 0x16, from USB stick to computer)</t>
+  </si>
+  <si>
+    <t>1-55</t>
+  </si>
+  <si>
+    <t>The Packed Link Key. This is run through an algorithm to become the 16-byte key that is used for encrypting and decrypting data</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BN54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1210,7 +1226,7 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:66" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -1488,10 +1504,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="42" t="s">
         <v>34</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>35</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
@@ -1622,10 +1638,10 @@
     </row>
     <row r="6" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
@@ -1633,10 +1649,10 @@
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
@@ -1644,22 +1660,22 @@
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
       <c r="C11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
@@ -1807,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BN45"/>
+  <dimension ref="A1:BN33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1824,14 +1840,14 @@
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -1861,9 +1877,9 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
@@ -1893,9 +1909,811 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
+    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="7"/>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7"/>
+      <c r="AR4" s="7"/>
+      <c r="AS4" s="7"/>
+      <c r="AT4" s="7"/>
+      <c r="AU4" s="7"/>
+      <c r="AV4" s="7"/>
+      <c r="AW4" s="7"/>
+      <c r="AX4" s="7"/>
+      <c r="AY4" s="7"/>
+      <c r="AZ4" s="7"/>
+      <c r="BA4" s="7"/>
+      <c r="BB4" s="7"/>
+      <c r="BC4" s="7"/>
+      <c r="BD4" s="7"/>
+      <c r="BE4" s="7"/>
+      <c r="BF4" s="7"/>
+      <c r="BG4" s="7"/>
+      <c r="BH4" s="7"/>
+      <c r="BI4" s="7"/>
+      <c r="BJ4" s="7"/>
+      <c r="BK4" s="7"/>
+      <c r="BL4" s="7"/>
+      <c r="BM4" s="7"/>
+      <c r="BN4" s="7"/>
+    </row>
+    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="7"/>
+      <c r="AR5" s="7"/>
+      <c r="AS5" s="7"/>
+      <c r="AT5" s="7"/>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="7"/>
+      <c r="AW5" s="7"/>
+      <c r="AX5" s="9"/>
+      <c r="AY5" s="7"/>
+      <c r="AZ5" s="9"/>
+      <c r="BA5" s="9"/>
+      <c r="BB5" s="7"/>
+      <c r="BC5" s="7"/>
+      <c r="BD5" s="7"/>
+      <c r="BE5" s="7"/>
+      <c r="BF5" s="7"/>
+      <c r="BG5" s="9"/>
+      <c r="BH5" s="7"/>
+      <c r="BI5" s="7"/>
+      <c r="BJ5" s="7"/>
+      <c r="BK5" s="7"/>
+      <c r="BL5" s="7"/>
+      <c r="BM5" s="7"/>
+      <c r="BN5" s="7"/>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6">
+        <v>7</v>
+      </c>
+      <c r="J6" s="6">
+        <v>8</v>
+      </c>
+      <c r="K6" s="6">
+        <v>9</v>
+      </c>
+      <c r="L6" s="6">
+        <v>10</v>
+      </c>
+      <c r="M6" s="5">
+        <v>11</v>
+      </c>
+      <c r="N6" s="5">
+        <v>12</v>
+      </c>
+      <c r="O6" s="5">
+        <v>13</v>
+      </c>
+      <c r="P6" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>15</v>
+      </c>
+      <c r="R6" s="5">
+        <v>16</v>
+      </c>
+      <c r="S6" s="5">
+        <v>17</v>
+      </c>
+      <c r="T6" s="5">
+        <v>18</v>
+      </c>
+      <c r="U6" s="6">
+        <v>19</v>
+      </c>
+      <c r="V6" s="6">
+        <v>20</v>
+      </c>
+      <c r="W6" s="6">
+        <v>21</v>
+      </c>
+      <c r="X6" s="6">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="37"/>
+      <c r="AE6" s="37"/>
+      <c r="AF6" s="37"/>
+      <c r="AG6" s="37"/>
+      <c r="AH6" s="37"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="37"/>
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="37"/>
+      <c r="AM6" s="37"/>
+      <c r="AN6" s="37"/>
+      <c r="AO6" s="37"/>
+      <c r="AP6" s="37"/>
+      <c r="AQ6" s="37"/>
+      <c r="AR6" s="37"/>
+      <c r="AS6" s="37"/>
+      <c r="AT6" s="37"/>
+      <c r="AU6" s="37"/>
+      <c r="AV6" s="37"/>
+      <c r="AW6" s="37"/>
+      <c r="AX6" s="37"/>
+      <c r="AY6" s="37"/>
+      <c r="AZ6" s="37"/>
+      <c r="BA6" s="37"/>
+      <c r="BB6" s="37"/>
+      <c r="BC6" s="37"/>
+      <c r="BD6" s="37"/>
+      <c r="BE6" s="37"/>
+      <c r="BF6" s="37"/>
+      <c r="BG6" s="37"/>
+      <c r="BH6" s="37"/>
+      <c r="BI6" s="37"/>
+      <c r="BJ6" s="37"/>
+      <c r="BK6" s="37"/>
+      <c r="BL6" s="37"/>
+      <c r="BM6" s="37"/>
+      <c r="BN6" s="37"/>
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="36"/>
+      <c r="AD7" s="36"/>
+      <c r="AE7" s="36"/>
+      <c r="AF7" s="36"/>
+      <c r="AG7" s="36"/>
+      <c r="AH7" s="36"/>
+      <c r="AI7" s="36"/>
+      <c r="AJ7" s="36"/>
+      <c r="AK7" s="36"/>
+      <c r="AL7" s="36"/>
+      <c r="AM7" s="36"/>
+      <c r="AN7" s="36"/>
+      <c r="AO7" s="36"/>
+      <c r="AP7" s="36"/>
+      <c r="AQ7" s="36"/>
+      <c r="AR7" s="36"/>
+      <c r="AS7" s="36"/>
+      <c r="AT7" s="36"/>
+      <c r="AU7" s="36"/>
+      <c r="AV7" s="36"/>
+      <c r="AW7" s="36"/>
+      <c r="AX7" s="36"/>
+      <c r="AY7" s="36"/>
+      <c r="AZ7" s="36"/>
+      <c r="BA7" s="36"/>
+      <c r="BB7" s="36"/>
+      <c r="BC7" s="36"/>
+      <c r="BD7" s="36"/>
+      <c r="BE7" s="36"/>
+      <c r="BF7" s="36"/>
+      <c r="BG7" s="36"/>
+      <c r="BH7" s="36"/>
+      <c r="BI7" s="36"/>
+      <c r="BJ7" s="36"/>
+      <c r="BK7" s="36"/>
+      <c r="BL7" s="36"/>
+      <c r="BM7" s="36"/>
+      <c r="BN7" s="36"/>
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="2"/>
+      <c r="BE8" s="2"/>
+      <c r="BF8" s="2"/>
+      <c r="BG8" s="2"/>
+      <c r="BH8" s="2"/>
+      <c r="BI8" s="2"/>
+      <c r="BJ8" s="2"/>
+      <c r="BK8" s="2"/>
+      <c r="BL8" s="2"/>
+      <c r="BM8" s="2"/>
+      <c r="BN8" s="2"/>
+    </row>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="B9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="B18" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C25" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C30" s="15"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M7:T7"/>
+    <mergeCell ref="U7:AB7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:BN45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="7"/>
+      <c r="AZ2" s="7"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="7"/>
+      <c r="BH2" s="7"/>
+      <c r="BI2" s="7"/>
+      <c r="BJ2" s="7"/>
+      <c r="BK2" s="7"/>
+      <c r="BL2" s="7"/>
+      <c r="BM2" s="7"/>
+      <c r="BN2" s="7"/>
+    </row>
+    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
+      <c r="AT3" s="7"/>
+      <c r="AU3" s="7"/>
+      <c r="AV3" s="7"/>
+      <c r="AW3" s="7"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
+      <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
+      <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
+      <c r="BK3" s="7"/>
+      <c r="BL3" s="7"/>
+      <c r="BM3" s="7"/>
+      <c r="BN3" s="7"/>
+    </row>
     <row r="4" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -2013,10 +2831,10 @@
         <v>18</v>
       </c>
       <c r="U6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V6" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="W6" s="38"/>
       <c r="X6" s="37"/>
@@ -2068,7 +2886,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="44"/>
@@ -2081,13 +2899,13 @@
         <v>10</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="M7" s="34" t="s">
         <v>16</v>
       </c>
       <c r="N7" s="46" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="O7" s="46"/>
       <c r="P7" s="46"/>
@@ -2211,10 +3029,10 @@
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
@@ -2222,10 +3040,10 @@
     </row>
     <row r="11" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2237,7 +3055,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2245,10 +3063,10 @@
     </row>
     <row r="15" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2256,58 +3074,58 @@
     </row>
     <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
       <c r="C18" s="20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
       <c r="C19" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="C20" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="C21" s="20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
       <c r="C22" s="20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="11"/>
       <c r="C23" s="20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="11"/>
       <c r="C24" s="20" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="11"/>
       <c r="C25" s="20" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2316,7 +3134,7 @@
     <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="11"/>
       <c r="C27" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2396,7 +3214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BN53"/>
   <sheetViews>
@@ -2415,12 +3233,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -2452,7 +3270,7 @@
     </row>
     <row r="3" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
@@ -2484,7 +3302,7 @@
     </row>
     <row r="4" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -2663,7 +3481,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>10</v>
@@ -2795,7 +3613,7 @@
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="39" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2930,10 +3748,10 @@
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
@@ -2941,10 +3759,10 @@
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
@@ -2955,7 +3773,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="2:66" x14ac:dyDescent="0.2">
@@ -2963,10 +3781,10 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
@@ -3107,7 +3925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BN43"/>
   <sheetViews>
@@ -3128,12 +3946,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -3165,7 +3983,7 @@
     </row>
     <row r="3" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
@@ -3197,7 +4015,7 @@
     </row>
     <row r="4" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -3363,10 +4181,10 @@
         <v>34</v>
       </c>
       <c r="AK6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL6" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="AL6" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="AM6" s="37"/>
       <c r="AN6" s="37"/>
@@ -3408,7 +4226,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
@@ -3418,7 +4236,7 @@
       <c r="K7" s="44"/>
       <c r="L7" s="44"/>
       <c r="M7" s="45" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N7" s="45"/>
       <c r="O7" s="45"/>
@@ -3428,19 +4246,19 @@
       <c r="S7" s="45"/>
       <c r="T7" s="45"/>
       <c r="U7" s="36" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="V7" s="36" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="W7" s="36" t="s">
         <v>7</v>
       </c>
       <c r="X7" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y7" s="46" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="Z7" s="46"/>
       <c r="AA7" s="46"/>
@@ -3553,10 +4371,10 @@
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
@@ -3564,10 +4382,10 @@
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
@@ -3575,10 +4393,10 @@
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
@@ -3587,10 +4405,10 @@
     </row>
     <row r="15" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3598,10 +4416,10 @@
     </row>
     <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3609,22 +4427,22 @@
     </row>
     <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="C20" s="20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="C21" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3739,12 +4557,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -3915,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -4050,40 +4868,40 @@
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
       <c r="C11" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
@@ -4092,7 +4910,7 @@
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:66" x14ac:dyDescent="0.2">
@@ -4101,7 +4919,7 @@
     <row r="16" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4420,12 +5238,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -4598,10 +5416,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -4735,10 +5553,10 @@
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
@@ -4747,10 +5565,10 @@
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
@@ -4774,7 +5592,7 @@
   <dimension ref="A1:BN60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4790,12 +5608,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -5063,10 +5881,10 @@
         <v>56</v>
       </c>
       <c r="BG4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="BH4" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="BH4" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="BI4"/>
       <c r="BJ4"/>
@@ -5179,7 +5997,7 @@
         <v>9</v>
       </c>
       <c r="AJ5" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AK5" s="42"/>
       <c r="AL5" s="42"/>
@@ -5281,10 +6099,10 @@
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
@@ -5293,10 +6111,10 @@
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
@@ -5304,10 +6122,10 @@
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
@@ -5315,10 +6133,10 @@
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
@@ -5326,64 +6144,64 @@
     </row>
     <row r="15" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
       <c r="C16" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" s="11"/>
       <c r="C17" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
       <c r="C18" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
       <c r="C19" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="C20" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="C21" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
       <c r="C22" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="11"/>
       <c r="C23" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="11"/>
       <c r="C24" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5394,10 +6212,10 @@
     <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5407,10 +6225,10 @@
     <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5421,10 +6239,10 @@
     <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5434,10 +6252,10 @@
     <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5448,10 +6266,10 @@
     <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="B34" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5680,7 +6498,7 @@
   <dimension ref="A1:BN67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5697,12 +6515,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -5964,16 +6782,16 @@
         <v>54</v>
       </c>
       <c r="BE4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="BF4" s="28" t="s">
-        <v>66</v>
-      </c>
       <c r="BG4" s="30" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BH4" s="30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="BI4"/>
       <c r="BJ4"/>
@@ -5987,13 +6805,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
@@ -6049,7 +6867,7 @@
       <c r="BE5" s="42"/>
       <c r="BF5" s="42"/>
       <c r="BG5" s="43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BH5" s="43"/>
       <c r="BI5"/>
@@ -6128,28 +6946,28 @@
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="8" t="s">
-        <v>94</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="8" t="s">
-        <v>95</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="8" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
@@ -6158,10 +6976,10 @@
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
@@ -6169,57 +6987,57 @@
     </row>
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B15" s="11"/>
       <c r="C15" s="21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
       <c r="C19" s="20"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C20" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6534,7 +7352,7 @@
   <dimension ref="B1:BN30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6550,12 +7368,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -6788,7 +7606,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
@@ -6923,34 +7741,34 @@
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
       <c r="C11" s="20" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
@@ -7035,7 +7853,7 @@
   <dimension ref="B1:BN27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7051,12 +7869,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -7088,7 +7906,7 @@
     </row>
     <row r="3" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
@@ -7120,7 +7938,7 @@
     </row>
     <row r="4" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -7223,7 +8041,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="32">
         <v>3</v>
@@ -7379,7 +8197,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
@@ -7393,7 +8211,7 @@
         <v>13</v>
       </c>
       <c r="K7" s="44" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="L7" s="44"/>
       <c r="M7" s="44"/>
@@ -7403,7 +8221,7 @@
       <c r="Q7" s="44"/>
       <c r="R7" s="44"/>
       <c r="S7" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T7" s="24" t="s">
         <v>2</v>
@@ -7421,16 +8239,16 @@
         <v>2</v>
       </c>
       <c r="Y7" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Z7" s="24" t="s">
         <v>2</v>
       </c>
       <c r="AA7" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AB7" s="45" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AC7" s="45"/>
       <c r="AD7" s="45"/>
@@ -7440,7 +8258,7 @@
       <c r="AH7" s="45"/>
       <c r="AI7" s="45"/>
       <c r="AJ7" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AK7" s="24" t="s">
         <v>2</v>
@@ -7464,7 +8282,7 @@
         <v>2</v>
       </c>
       <c r="AR7" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AS7" s="24"/>
       <c r="AT7" s="24"/>
@@ -7558,10 +8376,10 @@
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -7684,10 +8502,10 @@
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B11" s="26" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -7752,10 +8570,10 @@
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
@@ -7763,10 +8581,10 @@
     </row>
     <row r="15" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="2:66" x14ac:dyDescent="0.2">
@@ -7774,10 +8592,10 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
@@ -7785,10 +8603,10 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
@@ -7797,10 +8615,10 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
@@ -7842,10 +8660,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BN22"/>
+  <dimension ref="B1:BN20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7861,12 +8679,12 @@
   <sheetData>
     <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -8037,7 +8855,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
@@ -8047,7 +8865,7 @@
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
       <c r="K5" s="44" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="L5" s="44"/>
       <c r="M5" s="44"/>
@@ -8057,13 +8875,13 @@
       <c r="Q5" s="44"/>
       <c r="R5" s="44"/>
       <c r="S5" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V5" s="36"/>
       <c r="W5" s="36"/>
@@ -8180,15 +8998,15 @@
     </row>
     <row r="7" spans="2:66" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="2:66" x14ac:dyDescent="0.2">
@@ -8196,10 +9014,10 @@
     </row>
     <row r="10" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="2:66" x14ac:dyDescent="0.2">
@@ -8207,18 +9025,22 @@
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>51</v>
+        <v>185</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
     </row>
     <row r="14" spans="2:66" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="15" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B15" s="11"/>
@@ -8229,6 +9051,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="11"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
@@ -8236,19 +9059,11 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="C22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8258,17 +9073,17 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C4:U4 S5:U5" numberStoredAsText="1"/>
+    <ignoredError sqref="C4:U4 T5:U5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN33"/>
+  <dimension ref="B1:BN20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8282,14 +9097,14 @@
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
@@ -8319,10 +9134,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
+    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
       <c r="AP3" s="7"/>
@@ -8351,714 +9163,337 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="7"/>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="7"/>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="7"/>
-      <c r="BF4" s="7"/>
-      <c r="BG4" s="7"/>
-      <c r="BH4" s="7"/>
-      <c r="BI4" s="7"/>
-      <c r="BJ4" s="7"/>
-      <c r="BK4" s="7"/>
-      <c r="BL4" s="7"/>
-      <c r="BM4" s="7"/>
-      <c r="BN4" s="7"/>
-    </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="D5" s="13"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="7"/>
-      <c r="AR5" s="7"/>
-      <c r="AS5" s="7"/>
-      <c r="AT5" s="7"/>
-      <c r="AU5" s="7"/>
-      <c r="AV5" s="7"/>
-      <c r="AW5" s="7"/>
-      <c r="AX5" s="9"/>
-      <c r="AY5" s="7"/>
-      <c r="AZ5" s="9"/>
-      <c r="BA5" s="9"/>
-      <c r="BB5" s="7"/>
-      <c r="BC5" s="7"/>
-      <c r="BD5" s="7"/>
-      <c r="BE5" s="7"/>
-      <c r="BF5" s="7"/>
-      <c r="BG5" s="9"/>
-      <c r="BH5" s="7"/>
-      <c r="BI5" s="7"/>
-      <c r="BJ5" s="7"/>
-      <c r="BK5" s="7"/>
-      <c r="BL5" s="7"/>
-      <c r="BM5" s="7"/>
-      <c r="BN5" s="7"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D4" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F4" s="6">
         <v>4</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G4" s="6">
         <v>5</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H4" s="6">
         <v>6</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I4" s="6">
         <v>7</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J4" s="6">
         <v>8</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K4" s="6">
         <v>9</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L4" s="6">
         <v>10</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M4" s="6">
         <v>11</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N4" s="6">
         <v>12</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O4" s="6">
         <v>13</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P4" s="6">
         <v>14</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q4" s="6">
         <v>15</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R4" s="6">
         <v>16</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S4" s="6">
         <v>17</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T4" s="6">
         <v>18</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U4" s="6">
         <v>19</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V4" s="6">
         <v>20</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W4" s="6">
         <v>21</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X4" s="6">
         <v>22</v>
       </c>
-      <c r="Y6" s="6">
+      <c r="Y4" s="6">
         <v>23</v>
       </c>
-      <c r="Z6" s="6">
+      <c r="Z4" s="6">
         <v>24</v>
       </c>
-      <c r="AA6" s="6">
+      <c r="AA4" s="6">
         <v>25</v>
       </c>
-      <c r="AB6" s="6">
+      <c r="AB4" s="6">
         <v>26</v>
       </c>
-      <c r="AC6" s="37"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="37"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="37"/>
-      <c r="AH6" s="37"/>
-      <c r="AI6" s="38"/>
-      <c r="AJ6" s="37"/>
-      <c r="AK6" s="37"/>
-      <c r="AL6" s="37"/>
-      <c r="AM6" s="37"/>
-      <c r="AN6" s="37"/>
-      <c r="AO6" s="37"/>
-      <c r="AP6" s="37"/>
-      <c r="AQ6" s="37"/>
-      <c r="AR6" s="37"/>
-      <c r="AS6" s="37"/>
-      <c r="AT6" s="37"/>
-      <c r="AU6" s="37"/>
-      <c r="AV6" s="37"/>
-      <c r="AW6" s="37"/>
-      <c r="AX6" s="37"/>
-      <c r="AY6" s="37"/>
-      <c r="AZ6" s="37"/>
-      <c r="BA6" s="37"/>
-      <c r="BB6" s="37"/>
-      <c r="BC6" s="37"/>
-      <c r="BD6" s="37"/>
-      <c r="BE6" s="37"/>
-      <c r="BF6" s="37"/>
-      <c r="BG6" s="37"/>
-      <c r="BH6" s="37"/>
-      <c r="BI6" s="37"/>
-      <c r="BJ6" s="37"/>
-      <c r="BK6" s="37"/>
-      <c r="BL6" s="37"/>
-      <c r="BM6" s="37"/>
-      <c r="BN6" s="37"/>
-    </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="AC4" s="6">
+        <v>27</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="6">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>30</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>55</v>
+      </c>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="22"/>
+      <c r="AN4" s="22"/>
+      <c r="AO4" s="22"/>
+      <c r="AP4" s="22"/>
+      <c r="AQ4" s="22"/>
+      <c r="AR4" s="22"/>
+      <c r="AS4" s="22"/>
+      <c r="AT4" s="22"/>
+      <c r="AU4" s="22"/>
+      <c r="AV4" s="22"/>
+      <c r="AW4" s="22"/>
+      <c r="AX4" s="22"/>
+      <c r="AY4" s="22"/>
+      <c r="AZ4" s="22"/>
+      <c r="BA4" s="22"/>
+      <c r="BB4" s="22"/>
+      <c r="BC4" s="22"/>
+      <c r="BD4" s="22"/>
+      <c r="BE4" s="22"/>
+      <c r="BF4" s="22"/>
+      <c r="BG4" s="22"/>
+      <c r="BH4" s="22"/>
+      <c r="BI4" s="22"/>
+      <c r="BJ4" s="22"/>
+      <c r="BK4" s="22"/>
+      <c r="BL4" s="22"/>
+      <c r="BM4" s="22"/>
+      <c r="BN4" s="22"/>
+    </row>
+    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="V7" s="44"/>
-      <c r="W7" s="44"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="44"/>
-      <c r="Z7" s="44"/>
-      <c r="AA7" s="44"/>
-      <c r="AB7" s="44"/>
-      <c r="AC7" s="36"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="36"/>
-      <c r="AF7" s="36"/>
-      <c r="AG7" s="36"/>
-      <c r="AH7" s="36"/>
-      <c r="AI7" s="36"/>
-      <c r="AJ7" s="36"/>
-      <c r="AK7" s="36"/>
-      <c r="AL7" s="36"/>
-      <c r="AM7" s="36"/>
-      <c r="AN7" s="36"/>
-      <c r="AO7" s="36"/>
-      <c r="AP7" s="36"/>
-      <c r="AQ7" s="36"/>
-      <c r="AR7" s="36"/>
-      <c r="AS7" s="36"/>
-      <c r="AT7" s="36"/>
-      <c r="AU7" s="36"/>
-      <c r="AV7" s="36"/>
-      <c r="AW7" s="36"/>
-      <c r="AX7" s="36"/>
-      <c r="AY7" s="36"/>
-      <c r="AZ7" s="36"/>
-      <c r="BA7" s="36"/>
-      <c r="BB7" s="36"/>
-      <c r="BC7" s="36"/>
-      <c r="BD7" s="36"/>
-      <c r="BE7" s="36"/>
-      <c r="BF7" s="36"/>
-      <c r="BG7" s="36"/>
-      <c r="BH7" s="36"/>
-      <c r="BI7" s="36"/>
-      <c r="BJ7" s="36"/>
-      <c r="BK7" s="36"/>
-      <c r="BL7" s="36"/>
-      <c r="BM7" s="36"/>
-      <c r="BN7" s="36"/>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="2"/>
-      <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
-      <c r="AV8" s="2"/>
-      <c r="AW8" s="2"/>
-      <c r="AX8" s="2"/>
-      <c r="AY8" s="2"/>
-      <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
-      <c r="BB8" s="2"/>
-      <c r="BC8" s="2"/>
-      <c r="BD8" s="2"/>
-      <c r="BE8" s="2"/>
-      <c r="BF8" s="2"/>
-      <c r="BG8" s="2"/>
-      <c r="BH8" s="2"/>
-      <c r="BI8" s="2"/>
-      <c r="BJ8" s="2"/>
-      <c r="BK8" s="2"/>
-      <c r="BL8" s="2"/>
-      <c r="BM8" s="2"/>
-      <c r="BN8" s="2"/>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-    </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-    </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-    </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-    </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C25" s="8"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C31" s="8"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="8"/>
+      <c r="C5" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="42"/>
+      <c r="Y5" s="42"/>
+      <c r="Z5" s="42"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="42"/>
+      <c r="AE5" s="42"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="42"/>
+      <c r="AH5" s="42"/>
+      <c r="AI5" s="36"/>
+      <c r="AJ5" s="36"/>
+      <c r="AK5" s="36"/>
+      <c r="AL5" s="36"/>
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="36"/>
+      <c r="AO5" s="36"/>
+      <c r="AP5" s="36"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="36"/>
+      <c r="AS5" s="36"/>
+      <c r="AT5" s="36"/>
+      <c r="AU5" s="36"/>
+      <c r="AV5" s="36"/>
+      <c r="AW5" s="36"/>
+      <c r="AX5" s="36"/>
+      <c r="AY5" s="36"/>
+      <c r="AZ5" s="36"/>
+      <c r="BA5" s="36"/>
+      <c r="BB5" s="36"/>
+      <c r="BC5" s="36"/>
+      <c r="BD5" s="36"/>
+      <c r="BE5" s="36"/>
+      <c r="BF5" s="36"/>
+      <c r="BG5" s="36"/>
+      <c r="BH5" s="36"/>
+      <c r="BI5" s="36"/>
+      <c r="BJ5" s="36"/>
+      <c r="BK5" s="36"/>
+      <c r="BL5" s="36"/>
+      <c r="BM5" s="36"/>
+      <c r="BN5" s="36"/>
+    </row>
+    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
+      <c r="BE6" s="2"/>
+      <c r="BF6" s="2"/>
+      <c r="BG6" s="2"/>
+      <c r="BH6" s="2"/>
+      <c r="BI6" s="2"/>
+      <c r="BJ6" s="2"/>
+      <c r="BK6" s="2"/>
+      <c r="BL6" s="2"/>
+      <c r="BM6" s="2"/>
+      <c r="BN6" s="2"/>
+    </row>
+    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="C7" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B8" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+    </row>
+    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+    </row>
+    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="11"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="11"/>
+      <c r="C20" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="M7:T7"/>
-    <mergeCell ref="U7:AB7"/>
+  <mergeCells count="1">
+    <mergeCell ref="C5:AH5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
NEW FEATURE: stubs for decoding additional history events
</commit_message>
<xml_diff>
--- a/Bayer-Medtronic-640G USB HID Interface.xlsx
+++ b/Bayer-Medtronic-640G USB HID Interface.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28115"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennart/Documents/Remote Control Caty/decoding-contour-next-link/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Projects\pump_data_downloader\decoding_contour_next_link\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28280" windowHeight="16040" tabRatio="745" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28275" windowHeight="16035" tabRatio="745" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="USB Packets" sheetId="11" r:id="rId1"/>
@@ -25,12 +25,10 @@
     <sheet name="SEND_MESSAGE Request" sheetId="23" r:id="rId11"/>
     <sheet name="SEND_MESSAGE Response" sheetId="13" r:id="rId12"/>
     <sheet name="RECEIVE_MESSAGE" sheetId="24" r:id="rId13"/>
+    <sheet name="HISTORY_EVENTS" sheetId="27" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="249">
   <si>
     <t>Byte</t>
   </si>
@@ -694,6 +692,99 @@
   <si>
     <t>Pump serial number. For pumps older than the 640G, this returns a 6 digit ASCII serial number. For the NGP devices, it should be "000000"</t>
   </si>
+  <si>
+    <t>finalEstimate</t>
+  </si>
+  <si>
+    <t>estimateModifiedByUser</t>
+  </si>
+  <si>
+    <t>bolusStepSize</t>
+  </si>
+  <si>
+    <t>bolusWizardEstimate</t>
+  </si>
+  <si>
+    <t>activeInsulinCorrection</t>
+  </si>
+  <si>
+    <t>activeInsulin</t>
+  </si>
+  <si>
+    <t>foodEstimate</t>
+  </si>
+  <si>
+    <t>correctionEstimate</t>
+  </si>
+  <si>
+    <t>highBgTarget</t>
+  </si>
+  <si>
+    <t>lowBgTarget</t>
+  </si>
+  <si>
+    <t>carbRatio</t>
+  </si>
+  <si>
+    <t>isf</t>
+  </si>
+  <si>
+    <t>carbInput</t>
+  </si>
+  <si>
+    <t>bgInput</t>
+  </si>
+  <si>
+    <t>carbUnits</t>
+  </si>
+  <si>
+    <t>bgUnits</t>
+  </si>
+  <si>
+    <t>0x3D</t>
+  </si>
+  <si>
+    <t>BolusWizardEstimateEvent</t>
+  </si>
+  <si>
+    <t>programmedAmount</t>
+  </si>
+  <si>
+    <t>bNumber</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>NormalBolusProgrammed</t>
+  </si>
+  <si>
+    <t>deliveredAmount</t>
+  </si>
+  <si>
+    <t>0xDC</t>
+  </si>
+  <si>
+    <t>NormalBolusDelivered</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>event type</t>
+  </si>
+  <si>
+    <t>Contained by: MULTIPACKET_SEGMENT_TRANSMISSION as response to READ_HISTORY_REQUEST 0x0304</t>
+  </si>
 </sst>
 </file>
 
@@ -776,7 +867,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,6 +922,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -850,7 +953,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,6 +1068,25 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -980,6 +1102,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1276,24 +1401,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="6" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="44" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="52" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="59" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="66" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="44" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="52" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="59" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="66" width="3.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:66" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
@@ -1357,7 +1482,7 @@
       <c r="BL2" s="42"/>
       <c r="BM2" s="42"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1679,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1633,7 +1758,7 @@
       <c r="BM4" s="43"/>
       <c r="BN4" s="43"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1700,7 +1825,7 @@
       <c r="BM5" s="2"/>
       <c r="BN5" s="2"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
@@ -1708,10 +1833,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
@@ -1719,10 +1844,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>28</v>
       </c>
@@ -1730,149 +1855,149 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
       <c r="C42" s="8"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C46" s="8"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C48" s="8"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="14"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="8"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="8"/>
     </row>
   </sheetData>
@@ -1893,23 +2018,23 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -1941,7 +2066,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>99</v>
       </c>
@@ -1973,7 +2098,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>111</v>
       </c>
@@ -2005,7 +2130,7 @@
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="D5" s="12"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -2070,7 +2195,7 @@
       <c r="BM5" s="7"/>
       <c r="BN5" s="7"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -2191,7 +2316,7 @@
       <c r="BM6" s="36"/>
       <c r="BN6" s="36"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -2284,7 +2409,7 @@
       <c r="BM7" s="35"/>
       <c r="BN7" s="35"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2351,7 +2476,7 @@
       <c r="BM8" s="2"/>
       <c r="BN8" s="2"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>33</v>
       </c>
@@ -2359,7 +2484,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="16"/>
       <c r="C10" s="15"/>
@@ -2381,7 +2506,7 @@
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="16" t="s">
         <v>38</v>
@@ -2407,7 +2532,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="16"/>
       <c r="C12" s="18" t="s">
@@ -2431,7 +2556,7 @@
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="18" t="s">
@@ -2455,7 +2580,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="16"/>
       <c r="C14" s="18" t="s">
@@ -2479,7 +2604,7 @@
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16"/>
       <c r="C15" s="18" t="s">
@@ -2503,7 +2628,7 @@
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="16"/>
       <c r="C16" s="18" t="s">
@@ -2527,7 +2652,7 @@
       <c r="S16" s="15"/>
       <c r="T16" s="15"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="18"/>
@@ -2549,7 +2674,7 @@
       <c r="S17" s="15"/>
       <c r="T17" s="15"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="16" t="s">
         <v>119</v>
@@ -2575,7 +2700,7 @@
       <c r="S18" s="15"/>
       <c r="T18" s="15"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="16"/>
       <c r="C19" s="15"/>
@@ -2597,7 +2722,7 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="16" t="s">
         <v>165</v>
@@ -2623,7 +2748,7 @@
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="16"/>
       <c r="C21" s="15"/>
@@ -2645,7 +2770,7 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>166</v>
       </c>
@@ -2653,28 +2778,28 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C31" s="8"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
     </row>
   </sheetData>
@@ -2695,23 +2820,23 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -2743,7 +2868,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>129</v>
       </c>
@@ -2775,7 +2900,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>111</v>
       </c>
@@ -2807,7 +2932,7 @@
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="AN5" s="7"/>
       <c r="AO5" s="7"/>
       <c r="AP5" s="7"/>
@@ -2836,7 +2961,7 @@
       <c r="BM5" s="7"/>
       <c r="BN5" s="7"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +3070,7 @@
       <c r="BM6" s="36"/>
       <c r="BN6" s="36"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -3024,7 +3149,7 @@
       <c r="BM7"/>
       <c r="BN7"/>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="38"/>
       <c r="D8" s="2"/>
@@ -3091,7 +3216,7 @@
       <c r="BM8" s="2"/>
       <c r="BN8" s="2"/>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>161</v>
       </c>
@@ -3099,10 +3224,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>132</v>
       </c>
@@ -3110,11 +3235,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
@@ -3122,10 +3247,10 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>101</v>
       </c>
@@ -3133,10 +3258,10 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>136</v>
       </c>
@@ -3144,127 +3269,127 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="19" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="19" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="19" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
     </row>
-    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40"/>
       <c r="C40" s="14"/>
     </row>
-    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41"/>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42"/>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43"/>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45"/>
       <c r="C45" s="8"/>
     </row>
@@ -3284,23 +3409,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -3332,7 +3457,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>100</v>
       </c>
@@ -3364,7 +3489,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>123</v>
       </c>
@@ -3396,7 +3521,7 @@
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="AN5" s="7"/>
       <c r="AO5" s="7"/>
       <c r="AP5" s="7"/>
@@ -3425,7 +3550,7 @@
       <c r="BM5" s="7"/>
       <c r="BN5" s="7"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -3516,7 +3641,7 @@
       <c r="BM6" s="36"/>
       <c r="BN6" s="36"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -3607,7 +3732,7 @@
       <c r="BM7" s="35"/>
       <c r="BN7" s="35"/>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3674,7 +3799,7 @@
       <c r="BM8" s="2"/>
       <c r="BN8" s="2"/>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="38" t="s">
         <v>125</v>
@@ -3743,7 +3868,7 @@
       <c r="BM9" s="2"/>
       <c r="BN9" s="2"/>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3810,7 +3935,7 @@
       <c r="BM10" s="2"/>
       <c r="BN10" s="2"/>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>103</v>
       </c>
@@ -3818,10 +3943,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>126</v>
       </c>
@@ -3829,10 +3954,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
@@ -3840,10 +3965,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>101</v>
       </c>
@@ -3851,135 +3976,135 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
     </row>
-    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
     </row>
-    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
     </row>
-    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
     </row>
-    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
     </row>
-    <row r="45" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="10"/>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
     </row>
-    <row r="47" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48"/>
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49"/>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50"/>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51"/>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52"/>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53"/>
       <c r="C53" s="8"/>
     </row>
@@ -3997,23 +4122,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -4045,7 +4170,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>100</v>
       </c>
@@ -4077,7 +4202,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>140</v>
       </c>
@@ -4109,7 +4234,7 @@
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="AN5" s="7"/>
       <c r="AO5" s="7"/>
       <c r="AP5" s="7"/>
@@ -4138,7 +4263,7 @@
       <c r="BM5" s="7"/>
       <c r="BN5" s="7"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -4279,7 +4404,7 @@
       <c r="BM6" s="36"/>
       <c r="BN6" s="36"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -4366,7 +4491,7 @@
       <c r="BM7" s="35"/>
       <c r="BN7" s="35"/>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4433,7 +4558,7 @@
       <c r="BM8" s="2"/>
       <c r="BN8" s="2"/>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>103</v>
       </c>
@@ -4441,10 +4566,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>105</v>
       </c>
@@ -4452,10 +4577,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>120</v>
       </c>
@@ -4463,11 +4588,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>121</v>
       </c>
@@ -4475,10 +4600,10 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>102</v>
       </c>
@@ -4486,10 +4611,10 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>141</v>
       </c>
@@ -4497,97 +4622,97 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="19" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
     </row>
-    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38"/>
       <c r="C38" s="14"/>
     </row>
-    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39"/>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41"/>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42"/>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43"/>
       <c r="C43" s="8"/>
     </row>
@@ -4602,29 +4727,603 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BC9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(C4)-COLUMN($C4),2)</f>
+        <v>0x00</v>
+      </c>
+      <c r="D4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(D4)-COLUMN($C4),2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(E4)-COLUMN($C4),2)</f>
+        <v>0x02</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(F4)-COLUMN($C4),2)</f>
+        <v>0x03</v>
+      </c>
+      <c r="G4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(G4)-COLUMN($C4),2)</f>
+        <v>0x04</v>
+      </c>
+      <c r="H4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(H4)-COLUMN($C4),2)</f>
+        <v>0x05</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(I4)-COLUMN($C4),2)</f>
+        <v>0x06</v>
+      </c>
+      <c r="J4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(J4)-COLUMN($C4),2)</f>
+        <v>0x07</v>
+      </c>
+      <c r="K4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(K4)-COLUMN($C4),2)</f>
+        <v>0x08</v>
+      </c>
+      <c r="L4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(L4)-COLUMN($C4),2)</f>
+        <v>0x09</v>
+      </c>
+      <c r="M4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(M4)-COLUMN($C4),2)</f>
+        <v>0x0A</v>
+      </c>
+      <c r="N4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(N4)-COLUMN($C4),2)</f>
+        <v>0x0B</v>
+      </c>
+      <c r="O4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(O4)-COLUMN($C4),2)</f>
+        <v>0x0C</v>
+      </c>
+      <c r="P4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(P4)-COLUMN($C4),2)</f>
+        <v>0x0D</v>
+      </c>
+      <c r="Q4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(Q4)-COLUMN($C4),2)</f>
+        <v>0x0E</v>
+      </c>
+      <c r="R4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(R4)-COLUMN($C4),2)</f>
+        <v>0x0F</v>
+      </c>
+      <c r="S4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(S4)-COLUMN($C4),2)</f>
+        <v>0x10</v>
+      </c>
+      <c r="T4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(T4)-COLUMN($C4),2)</f>
+        <v>0x11</v>
+      </c>
+      <c r="U4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(U4)-COLUMN($C4),2)</f>
+        <v>0x12</v>
+      </c>
+      <c r="V4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(V4)-COLUMN($C4),2)</f>
+        <v>0x13</v>
+      </c>
+      <c r="W4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(W4)-COLUMN($C4),2)</f>
+        <v>0x14</v>
+      </c>
+      <c r="X4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(X4)-COLUMN($C4),2)</f>
+        <v>0x15</v>
+      </c>
+      <c r="Y4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(Y4)-COLUMN($C4),2)</f>
+        <v>0x16</v>
+      </c>
+      <c r="Z4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(Z4)-COLUMN($C4),2)</f>
+        <v>0x17</v>
+      </c>
+      <c r="AA4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AA4)-COLUMN($C4),2)</f>
+        <v>0x18</v>
+      </c>
+      <c r="AB4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AB4)-COLUMN($C4),2)</f>
+        <v>0x19</v>
+      </c>
+      <c r="AC4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AC4)-COLUMN($C4),2)</f>
+        <v>0x1A</v>
+      </c>
+      <c r="AD4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AD4)-COLUMN($C4),2)</f>
+        <v>0x1B</v>
+      </c>
+      <c r="AE4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AE4)-COLUMN($C4),2)</f>
+        <v>0x1C</v>
+      </c>
+      <c r="AF4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AF4)-COLUMN($C4),2)</f>
+        <v>0x1D</v>
+      </c>
+      <c r="AG4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AG4)-COLUMN($C4),2)</f>
+        <v>0x1E</v>
+      </c>
+      <c r="AH4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AH4)-COLUMN($C4),2)</f>
+        <v>0x1F</v>
+      </c>
+      <c r="AI4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AI4)-COLUMN($C4),2)</f>
+        <v>0x20</v>
+      </c>
+      <c r="AJ4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AJ4)-COLUMN($C4),2)</f>
+        <v>0x21</v>
+      </c>
+      <c r="AK4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AK4)-COLUMN($C4),2)</f>
+        <v>0x22</v>
+      </c>
+      <c r="AL4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AL4)-COLUMN($C4),2)</f>
+        <v>0x23</v>
+      </c>
+      <c r="AM4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AM4)-COLUMN($C4),2)</f>
+        <v>0x24</v>
+      </c>
+      <c r="AN4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AN4)-COLUMN($C4),2)</f>
+        <v>0x25</v>
+      </c>
+      <c r="AO4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AO4)-COLUMN($C4),2)</f>
+        <v>0x26</v>
+      </c>
+      <c r="AP4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AP4)-COLUMN($C4),2)</f>
+        <v>0x27</v>
+      </c>
+      <c r="AQ4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AQ4)-COLUMN($C4),2)</f>
+        <v>0x28</v>
+      </c>
+      <c r="AR4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AR4)-COLUMN($C4),2)</f>
+        <v>0x29</v>
+      </c>
+      <c r="AS4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AS4)-COLUMN($C4),2)</f>
+        <v>0x2A</v>
+      </c>
+      <c r="AT4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AT4)-COLUMN($C4),2)</f>
+        <v>0x2B</v>
+      </c>
+      <c r="AU4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AU4)-COLUMN($C4),2)</f>
+        <v>0x2C</v>
+      </c>
+      <c r="AV4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AV4)-COLUMN($C4),2)</f>
+        <v>0x2D</v>
+      </c>
+      <c r="AW4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AW4)-COLUMN($C4),2)</f>
+        <v>0x2E</v>
+      </c>
+      <c r="AX4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AX4)-COLUMN($C4),2)</f>
+        <v>0x2F</v>
+      </c>
+      <c r="AY4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AY4)-COLUMN($C4),2)</f>
+        <v>0x30</v>
+      </c>
+      <c r="AZ4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(AZ4)-COLUMN($C4),2)</f>
+        <v>0x31</v>
+      </c>
+      <c r="BA4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(BA4)-COLUMN($C4),2)</f>
+        <v>0x32</v>
+      </c>
+      <c r="BB4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(BB4)-COLUMN($C4),2)</f>
+        <v>0x33</v>
+      </c>
+      <c r="BC4" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(COLUMN(BC4)-COLUMN($C4),2)</f>
+        <v>0x34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="54"/>
+      <c r="AJ5" s="54"/>
+      <c r="AK5" s="54"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="17"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" t="s">
+        <v>243</v>
+      </c>
+      <c r="N6" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="O6" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="P6" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q6" s="52" t="s">
+        <v>236</v>
+      </c>
+      <c r="R6" s="52"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="52"/>
+      <c r="U6" s="49" t="s">
+        <v>242</v>
+      </c>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z6" s="52"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="N7" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="O7" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="P7" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q7" s="52" t="s">
+        <v>236</v>
+      </c>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
+      <c r="U7" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P8" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="S8" s="49"/>
+      <c r="T8" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="U8" s="50"/>
+      <c r="V8" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="49" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50"/>
+      <c r="AG8" s="50"/>
+      <c r="AH8" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="50"/>
+      <c r="AO8" s="50"/>
+      <c r="AP8" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="AQ8" s="49"/>
+      <c r="AR8" s="49"/>
+      <c r="AS8" s="49"/>
+      <c r="AT8" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="AU8" s="50"/>
+      <c r="AV8" s="50"/>
+      <c r="AW8" s="50"/>
+      <c r="AX8" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AY8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ8" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="BA8" s="49"/>
+      <c r="BB8" s="49"/>
+      <c r="BC8" s="49"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="C9" s="48"/>
+      <c r="N9" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AT8:AW8"/>
+    <mergeCell ref="AZ8:BC8"/>
+    <mergeCell ref="AH8:AK8"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="AD8:AG8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="Q7:T7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>60</v>
       </c>
@@ -4656,7 +5355,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -4721,7 +5420,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -4792,7 +5491,7 @@
       <c r="BM4"/>
       <c r="BN4"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -4863,7 +5562,7 @@
       <c r="BM5"/>
       <c r="BN5"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -4930,7 +5629,7 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
@@ -4938,120 +5637,120 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="C9" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18" s="10"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20" s="10"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22" s="10"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24" s="10"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="10"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="10"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="10"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="10"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="16"/>
       <c r="C31" s="15"/>
@@ -5073,7 +5772,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="16"/>
       <c r="C32" s="18"/>
@@ -5095,7 +5794,7 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="16"/>
       <c r="C33" s="18"/>
@@ -5117,7 +5816,7 @@
       <c r="S33" s="15"/>
       <c r="T33" s="15"/>
     </row>
-    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="16"/>
       <c r="C34" s="18"/>
@@ -5139,7 +5838,7 @@
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
     </row>
-    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="16"/>
       <c r="C35" s="15"/>
@@ -5161,7 +5860,7 @@
       <c r="S35" s="15"/>
       <c r="T35" s="15"/>
     </row>
-    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="16"/>
       <c r="C36" s="18"/>
@@ -5183,7 +5882,7 @@
       <c r="S36" s="15"/>
       <c r="T36" s="15"/>
     </row>
-    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="16"/>
       <c r="C37" s="15"/>
@@ -5205,74 +5904,74 @@
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
     </row>
-    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38" s="10"/>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39" s="10"/>
     </row>
-    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41" s="10"/>
     </row>
-    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42" s="10"/>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43" s="10"/>
     </row>
-    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44" s="10"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46" s="10"/>
       <c r="C46" s="8"/>
     </row>
-    <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48" s="8"/>
     </row>
-    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54" s="8"/>
     </row>
-    <row r="56" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56" s="8"/>
@@ -5289,23 +5988,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>60</v>
       </c>
@@ -5337,7 +6036,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -5402,7 +6101,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -5475,7 +6174,7 @@
       <c r="BM4"/>
       <c r="BN4"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -5548,7 +6247,7 @@
       <c r="BM5"/>
       <c r="BN5"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -5615,7 +6314,7 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
@@ -5623,11 +6322,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>38</v>
       </c>
@@ -5635,14 +6334,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
   </sheetData>
@@ -5655,27 +6354,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="58" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>63</v>
       </c>
@@ -5707,7 +6406,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -5772,7 +6471,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -5957,7 +6656,7 @@
       <c r="BM4"/>
       <c r="BN4"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -6094,7 +6793,7 @@
       <c r="BM5"/>
       <c r="BN5"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -6161,7 +6860,7 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
@@ -6169,11 +6868,11 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>38</v>
       </c>
@@ -6181,28 +6880,28 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="8" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="8" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>39</v>
       </c>
@@ -6210,10 +6909,10 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>45</v>
       </c>
@@ -6221,10 +6920,10 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>47</v>
       </c>
@@ -6232,66 +6931,66 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="10"/>
       <c r="C28" s="19"/>
     </row>
-    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="10" t="s">
         <v>48</v>
@@ -6300,11 +6999,11 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="10" t="s">
         <v>49</v>
@@ -6313,12 +7012,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="10"/>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33" s="10" t="s">
         <v>180</v>
@@ -6327,11 +7026,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35" s="10" t="s">
         <v>179</v>
@@ -6340,11 +7039,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37" s="10" t="s">
         <v>17</v>
@@ -6353,12 +7052,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38" s="10"/>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39" s="10" t="s">
         <v>85</v>
@@ -6367,12 +7066,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41"/>
       <c r="C41" s="14"/>
@@ -6394,7 +7093,7 @@
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
       <c r="B42" s="16"/>
       <c r="C42" s="8"/>
@@ -6416,7 +7115,7 @@
       <c r="S42" s="15"/>
       <c r="T42" s="15"/>
     </row>
-    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="16"/>
       <c r="C43" s="18"/>
@@ -6438,7 +7137,7 @@
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
     </row>
-    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="16"/>
       <c r="C44" s="15"/>
@@ -6460,7 +7159,7 @@
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
     </row>
-    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="16"/>
       <c r="C45" s="18"/>
@@ -6482,7 +7181,7 @@
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
     </row>
-    <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="16"/>
       <c r="C46" s="15"/>
@@ -6504,74 +7203,74 @@
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
     </row>
-    <row r="47" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47" s="10"/>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48" s="10"/>
     </row>
-    <row r="49" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49" s="10"/>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50" s="10"/>
     </row>
-    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51" s="10"/>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52" s="10"/>
     </row>
-    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53" s="10"/>
       <c r="C53" s="8"/>
     </row>
-    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55" s="10"/>
       <c r="C55" s="8"/>
     </row>
-    <row r="57" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="59" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63" s="8"/>
     </row>
-    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65" s="8"/>
@@ -6596,24 +7295,24 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="3" style="1" customWidth="1"/>
     <col min="4" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="58" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>81</v>
       </c>
@@ -6645,7 +7344,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -6710,7 +7409,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -6895,7 +7594,7 @@
       <c r="BM4"/>
       <c r="BN4"/>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -6972,7 +7671,7 @@
       <c r="BM5"/>
       <c r="BN5"/>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -7039,7 +7738,7 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
@@ -7047,7 +7746,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
@@ -23435,7 +24134,7 @@
       <c r="XFC8" s="8"/>
       <c r="XFD8" s="8"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
@@ -39823,83 +40522,83 @@
       <c r="XFC9" s="8"/>
       <c r="XFD9" s="8"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
       <c r="C13" s="8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
       <c r="C15" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>38</v>
       </c>
@@ -39907,10 +40606,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>84</v>
       </c>
@@ -39918,16 +40617,16 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>62</v>
       </c>
@@ -39998,7 +40697,7 @@
       <c r="BM28"/>
       <c r="BN28"/>
     </row>
-    <row r="29" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>90</v>
       </c>
@@ -40069,7 +40768,7 @@
       <c r="BM29"/>
       <c r="BN29"/>
     </row>
-    <row r="30" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="19"/>
       <c r="D30"/>
@@ -40136,7 +40835,7 @@
       <c r="BM30"/>
       <c r="BN30"/>
     </row>
-    <row r="31" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:66" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
         <v>91</v>
       </c>
@@ -40204,7 +40903,7 @@
       <c r="BM31"/>
       <c r="BN31"/>
     </row>
-    <row r="32" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:66" x14ac:dyDescent="0.25">
       <c r="C32" s="14" t="s">
         <v>95</v>
       </c>
@@ -40272,7 +40971,7 @@
       <c r="BM32"/>
       <c r="BN32"/>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
       <c r="C33" s="14"/>
       <c r="D33"/>
       <c r="E33"/>
@@ -40338,7 +41037,7 @@
       <c r="BM33"/>
       <c r="BN33"/>
     </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
       <c r="C34" s="8" t="s">
         <v>92</v>
       </c>
@@ -40406,97 +41105,97 @@
       <c r="BM34"/>
       <c r="BN34"/>
     </row>
-    <row r="35" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35"/>
     </row>
-    <row r="36" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36"/>
     </row>
-    <row r="37" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37"/>
     </row>
-    <row r="38" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38" s="10"/>
       <c r="C38" s="19"/>
     </row>
-    <row r="39" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39" s="10"/>
       <c r="C39" s="19"/>
     </row>
-    <row r="40" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="10"/>
       <c r="C40" s="19"/>
     </row>
-    <row r="41" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41" s="10"/>
       <c r="C41" s="19"/>
     </row>
-    <row r="42" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42" s="10"/>
       <c r="C42" s="19"/>
     </row>
-    <row r="43" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43" s="10"/>
       <c r="C43" s="19"/>
     </row>
-    <row r="44" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44" s="10"/>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46" s="10"/>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47" s="10"/>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:66" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48" s="10"/>
       <c r="C48" s="8"/>
     </row>
-    <row r="49" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49" s="10"/>
     </row>
-    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50" s="10"/>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51" s="10"/>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52" s="10"/>
       <c r="C52" s="20"/>
     </row>
-    <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53" s="10"/>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54"/>
       <c r="C54" s="14"/>
@@ -40518,7 +41217,7 @@
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
     </row>
-    <row r="55" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17"/>
       <c r="B55" s="16"/>
       <c r="C55" s="8"/>
@@ -40540,7 +41239,7 @@
       <c r="S55" s="15"/>
       <c r="T55" s="15"/>
     </row>
-    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17"/>
       <c r="B56" s="16"/>
       <c r="C56" s="18"/>
@@ -40562,7 +41261,7 @@
       <c r="S56" s="15"/>
       <c r="T56" s="15"/>
     </row>
-    <row r="57" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
       <c r="B57" s="16"/>
       <c r="C57" s="15"/>
@@ -40584,7 +41283,7 @@
       <c r="S57" s="15"/>
       <c r="T57" s="15"/>
     </row>
-    <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17"/>
       <c r="B58" s="16"/>
       <c r="C58" s="18"/>
@@ -40606,7 +41305,7 @@
       <c r="S58" s="15"/>
       <c r="T58" s="15"/>
     </row>
-    <row r="59" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="17"/>
       <c r="B59" s="16"/>
       <c r="C59" s="15"/>
@@ -40628,74 +41327,74 @@
       <c r="S59" s="15"/>
       <c r="T59" s="15"/>
     </row>
-    <row r="60" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60" s="10"/>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61" s="10"/>
     </row>
-    <row r="62" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62" s="10"/>
       <c r="C62" s="8"/>
     </row>
-    <row r="63" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63" s="10"/>
     </row>
-    <row r="64" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64" s="10"/>
       <c r="C64" s="8"/>
     </row>
-    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65" s="10"/>
     </row>
-    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66" s="10"/>
       <c r="C66" s="8"/>
     </row>
-    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68" s="10"/>
       <c r="C68" s="8"/>
     </row>
-    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70" s="8"/>
     </row>
-    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72" s="8"/>
     </row>
-    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73" s="8"/>
     </row>
-    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74" s="8"/>
     </row>
-    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75" s="14"/>
     </row>
-    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76" s="8"/>
     </row>
-    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78" s="8"/>
@@ -40721,23 +41420,23 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>64</v>
       </c>
@@ -40769,7 +41468,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -40834,7 +41533,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -40967,7 +41666,7 @@
       <c r="BM4"/>
       <c r="BN4"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -41038,7 +41737,7 @@
       <c r="BM5"/>
       <c r="BN5"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -41105,7 +41804,7 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>65</v>
       </c>
@@ -41113,96 +41812,96 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="C9" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="19" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="19" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
     </row>
   </sheetData>
@@ -41222,23 +41921,23 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -41270,7 +41969,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>100</v>
       </c>
@@ -41302,7 +42001,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>98</v>
       </c>
@@ -41334,7 +42033,7 @@
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="D5" s="12"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -41399,7 +42098,7 @@
       <c r="BM5" s="7"/>
       <c r="BN5" s="7"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>0</v>
       </c>
@@ -41552,7 +42251,7 @@
       <c r="BM6" s="33"/>
       <c r="BN6" s="33"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>1</v>
       </c>
@@ -41669,7 +42368,7 @@
       <c r="BM7" s="23"/>
       <c r="BN7" s="23"/>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="39"/>
       <c r="C8" s="40"/>
       <c r="D8" s="23"/>
@@ -41736,7 +42435,7 @@
       <c r="BM8" s="2"/>
       <c r="BN8" s="2"/>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>103</v>
       </c>
@@ -41801,7 +42500,7 @@
       <c r="BG9" s="26"/>
       <c r="BH9" s="26"/>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="25"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -41862,7 +42561,7 @@
       <c r="BG10" s="26"/>
       <c r="BH10" s="26"/>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>105</v>
       </c>
@@ -41927,10 +42626,10 @@
       <c r="BG11" s="26"/>
       <c r="BH11" s="26"/>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>199</v>
       </c>
@@ -41938,10 +42637,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>157</v>
       </c>
@@ -41949,10 +42648,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>202</v>
       </c>
@@ -41960,10 +42659,10 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>203</v>
       </c>
@@ -41971,11 +42670,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>204</v>
       </c>
@@ -41983,10 +42682,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>159</v>
       </c>
@@ -41994,11 +42693,11 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>206</v>
       </c>
@@ -42006,11 +42705,11 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>209</v>
       </c>
@@ -42018,11 +42717,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>20</v>
       </c>
@@ -42030,20 +42729,20 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="41" t="s">
         <v>210</v>
       </c>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="30">
         <v>1</v>
@@ -42121,7 +42820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="23" t="s">
         <v>2</v>
@@ -42199,7 +42898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="8"/>
     </row>
@@ -42225,23 +42924,23 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>109</v>
       </c>
@@ -42273,7 +42972,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
       <c r="AP3" s="7"/>
@@ -42302,7 +43001,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -42409,7 +43108,7 @@
       <c r="BM4" s="21"/>
       <c r="BN4" s="21"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -42488,7 +43187,7 @@
       <c r="BM5" s="35"/>
       <c r="BN5" s="35"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -42555,12 +43254,12 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>161</v>
       </c>
@@ -42568,10 +43267,10 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>157</v>
       </c>
@@ -42579,10 +43278,10 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>170</v>
       </c>
@@ -42590,10 +43289,10 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>47</v>
       </c>
@@ -42601,26 +43300,26 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="8"/>
     </row>
@@ -42645,23 +43344,23 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="44" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="52" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="66" width="3" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>174</v>
       </c>
@@ -42693,7 +43392,7 @@
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
     </row>
-    <row r="3" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="AN3" s="7"/>
       <c r="AO3" s="7"/>
       <c r="AP3" s="7"/>
@@ -42722,7 +43421,7 @@
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
     </row>
-    <row r="4" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -42855,7 +43554,7 @@
       <c r="BM4" s="21"/>
       <c r="BN4" s="21"/>
     </row>
-    <row r="5" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -42926,7 +43625,7 @@
       <c r="BM5" s="35"/>
       <c r="BN5" s="35"/>
     </row>
-    <row r="6" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -42993,12 +43692,12 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="2"/>
     </row>
-    <row r="7" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>175</v>
       </c>
@@ -43006,47 +43705,47 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="2:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="8"/>
     </row>

</xml_diff>